<commit_message>
modify frontend for new data
</commit_message>
<xml_diff>
--- a/insuranceApp/backend/datas/医疗保险.xlsx
+++ b/insuranceApp/backend/datas/医疗保险.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\desktop\数据\最终数据集\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729204BF-155C-4765-8BB6-BA8491DB8E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A9C0EB-51C3-483D-A261-F6C32F556048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6400" yWindow="120" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="医疗保险数据_同结构清洗v2" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>product_name</t>
   </si>
   <si>
-    <t>医疗保险具体产品名称</t>
-  </si>
-  <si>
     <t>VARCHAR(63)</t>
   </si>
   <si>
@@ -709,6 +706,10 @@
   </si>
   <si>
     <t>{"20000" : "固定数额: 非特定康复医疗", "0" : "固定数额: 特定康复医疗"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>产品名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1267,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.36328125" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -1293,10 +1294,10 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1366,153 +1367,153 @@
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="N3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="U3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -1577,66 +1578,66 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="L5" s="3" t="s">
+      <c r="O5" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="P5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S5" s="1" t="s">
+      <c r="V5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="T5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U5" s="1" t="s">
+      <c r="W5" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="W5" s="3" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -1701,13 +1702,13 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -1772,84 +1773,84 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" s="1">
         <v>7.6999999999999999E-2</v>
@@ -1914,13 +1915,13 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1">
         <v>60</v>
@@ -1985,13 +1986,13 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" s="1">
         <v>30</v>
@@ -2056,13 +2057,13 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -2127,13 +2128,13 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>109</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -2159,45 +2160,45 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="H14" s="1" t="s">
+      <c r="N14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="S14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="S14" s="1" t="s">
+      <c r="T14" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="U14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="T14" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="U14" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="V14" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -2206,10 +2207,10 @@
         <v>0</v>
       </c>
       <c r="S15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T15" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="U15" s="1">
         <v>0</v>
@@ -2223,124 +2224,124 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N16" s="1">
         <v>0</v>
       </c>
       <c r="S16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="T16" s="1" t="s">
+      <c r="U16" s="1">
+        <v>0</v>
+      </c>
+      <c r="V16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="U16" s="1">
-        <v>0</v>
-      </c>
-      <c r="V16" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="W16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="O17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="R17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
@@ -2372,13 +2373,13 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -2410,41 +2411,41 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E23" s="1">
         <v>1</v>
@@ -2452,13 +2453,13 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
@@ -2466,13 +2467,13 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>123</v>
-      </c>
       <c r="C25" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -2492,13 +2493,13 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D26" s="1">
         <v>0.8</v>
@@ -2515,91 +2516,91 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="H27" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O27" s="1">
         <v>0</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="H28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O28" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="O28" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O29" s="1">
         <v>0</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D30" s="1">
         <v>100</v>
@@ -2619,13 +2620,13 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E31" s="1">
         <v>400</v>
@@ -2669,63 +2670,63 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="O32" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="R32" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S32" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T32" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U32" s="1">
         <v>1</v>
       </c>
       <c r="V32" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
@@ -2769,60 +2770,60 @@
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="F34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="T34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="U34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>137</v>
-      </c>
       <c r="C35" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E35" s="1">
         <v>14</v>
@@ -2851,13 +2852,13 @@
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>139</v>
-      </c>
       <c r="C36" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E36" s="1">
         <v>400</v>
@@ -2886,13 +2887,13 @@
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E37" s="1">
         <v>0</v>
@@ -2921,13 +2922,13 @@
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E38" s="1">
         <v>1</v>
@@ -2956,48 +2957,48 @@
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -3056,30 +3057,30 @@
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M41" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="P41" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M42" s="1">
         <v>400</v>
@@ -3090,13 +3091,13 @@
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M43" s="1">
         <v>0</v>
@@ -3107,16 +3108,16 @@
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P44" s="1">
         <v>1</v>
@@ -3124,30 +3125,30 @@
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D46" s="1">
         <v>0</v>
@@ -3212,13 +3213,13 @@
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D47" s="1">
         <v>0</v>
@@ -3283,13 +3284,13 @@
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D48" s="1">
         <v>0</v>
@@ -3354,13 +3355,13 @@
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D49" s="1">
         <v>0</v>
@@ -3425,13 +3426,13 @@
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D50" s="1">
         <v>0</v>
@@ -3496,13 +3497,13 @@
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D51" s="1">
         <v>0</v>
@@ -3567,13 +3568,13 @@
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D52" s="1">
         <v>0</v>
@@ -3638,33 +3639,33 @@
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N53" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D54" s="1">
         <v>0</v>
@@ -3729,13 +3730,13 @@
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D55" s="1">
         <v>0</v>
@@ -3800,13 +3801,13 @@
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D56" s="1">
         <v>0</v>
@@ -3871,13 +3872,13 @@
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D57" s="1">
         <v>0</v>
@@ -3942,13 +3943,13 @@
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D58" s="1">
         <v>0</v>
@@ -4013,13 +4014,13 @@
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D59" s="1">
         <v>0</v>
@@ -4084,13 +4085,13 @@
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D60" s="1">
         <v>0</v>
@@ -4155,13 +4156,13 @@
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D61" s="1">
         <v>0</v>
@@ -4226,78 +4227,78 @@
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D62" s="1" t="s">
+      <c r="E62" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I62" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="J62" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F62" s="1" t="s">
+      <c r="K62" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G62" s="1" t="s">
+      <c r="L62" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H62" s="1" t="s">
+      <c r="M62" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I62" s="1" t="s">
+      <c r="N62" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J62" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K62" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="L62" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="M62" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="N62" s="1" t="s">
+      <c r="O62" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O62" s="1" t="s">
+      <c r="P62" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="P62" s="1" t="s">
+      <c r="Q62" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q62" s="1" t="s">
+      <c r="R62" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="S62" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="R62" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="S62" s="1" t="s">
+      <c r="T62" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="U62" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="T62" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="U62" s="1" t="s">
+      <c r="V62" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="W62" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="V62" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="W62" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>